<commit_message>
Some schematic updates, spi test is working
</commit_message>
<xml_diff>
--- a/RCS/INTEVLogger Bill of Materials.xlsx
+++ b/RCS/INTEVLogger Bill of Materials.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13584" windowHeight="6384"/>
+    <workbookView xWindow="936" yWindow="0" windowWidth="13584" windowHeight="6384"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -187,7 +187,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -385,6 +385,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -420,6 +437,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -598,8 +632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>